<commit_message>
Update web reports - 2025-10-09 20:45:33
</commit_message>
<xml_diff>
--- a/quickbook_summary.xlsx
+++ b/quickbook_summary.xlsx
@@ -2308,7 +2308,7 @@
         </is>
       </c>
       <c r="G45" s="3" t="n">
-        <v>-345</v>
+        <v>345</v>
       </c>
     </row>
     <row r="46">
@@ -3373,7 +3373,7 @@
         </is>
       </c>
       <c r="G78" s="3" t="n">
-        <v>-2133.85</v>
+        <v>2133.85</v>
       </c>
     </row>
     <row r="79">
@@ -3633,7 +3633,7 @@
         </is>
       </c>
       <c r="G86" s="3" t="n">
-        <v>-2133.85</v>
+        <v>2133.85</v>
       </c>
     </row>
     <row r="87">
@@ -5403,7 +5403,7 @@
         </is>
       </c>
       <c r="G140" s="3" t="n">
-        <v>-185.57</v>
+        <v>185.57</v>
       </c>
     </row>
     <row r="141">
@@ -5436,7 +5436,7 @@
         </is>
       </c>
       <c r="G141" s="3" t="n">
-        <v>-50</v>
+        <v>50</v>
       </c>
     </row>
     <row r="142">
@@ -5667,7 +5667,7 @@
         </is>
       </c>
       <c r="G148" s="3" t="n">
-        <v>-180</v>
+        <v>180</v>
       </c>
     </row>
     <row r="149">
@@ -9756,7 +9756,7 @@
         </is>
       </c>
       <c r="G273" s="3" t="n">
-        <v>-2573.41</v>
+        <v>2573.41</v>
       </c>
     </row>
     <row r="274">
@@ -9789,7 +9789,7 @@
         </is>
       </c>
       <c r="G274" s="3" t="n">
-        <v>-199.44</v>
+        <v>199.44</v>
       </c>
     </row>
     <row r="275">
@@ -10412,7 +10412,7 @@
         </is>
       </c>
       <c r="G293" s="3" t="n">
-        <v>-265.28</v>
+        <v>265.28</v>
       </c>
     </row>
     <row r="294">
@@ -10445,7 +10445,7 @@
         </is>
       </c>
       <c r="G294" s="3" t="n">
-        <v>-26.46</v>
+        <v>26.46</v>
       </c>
     </row>
     <row r="295">
@@ -10478,7 +10478,7 @@
         </is>
       </c>
       <c r="G295" s="3" t="n">
-        <v>-2.16</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="296">
@@ -10511,7 +10511,7 @@
         </is>
       </c>
       <c r="G296" s="3" t="n">
-        <v>-22.94</v>
+        <v>22.94</v>
       </c>
     </row>
     <row r="297">
@@ -10544,7 +10544,7 @@
         </is>
       </c>
       <c r="G297" s="3" t="n">
-        <v>-755.66</v>
+        <v>755.66</v>
       </c>
     </row>
     <row r="298">
@@ -10577,7 +10577,7 @@
         </is>
       </c>
       <c r="G298" s="3" t="n">
-        <v>-33.44</v>
+        <v>33.44</v>
       </c>
     </row>
     <row r="299">
@@ -10610,7 +10610,7 @@
         </is>
       </c>
       <c r="G299" s="3" t="n">
-        <v>-7.86</v>
+        <v>7.86</v>
       </c>
     </row>
     <row r="300">
@@ -10643,7 +10643,7 @@
         </is>
       </c>
       <c r="G300" s="3" t="n">
-        <v>-24.97</v>
+        <v>24.97</v>
       </c>
     </row>
     <row r="301">
@@ -10676,7 +10676,7 @@
         </is>
       </c>
       <c r="G301" s="3" t="n">
-        <v>-21.7</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="302">
@@ -10709,7 +10709,7 @@
         </is>
       </c>
       <c r="G302" s="3" t="n">
-        <v>-10.85</v>
+        <v>10.85</v>
       </c>
     </row>
     <row r="303">
@@ -10742,7 +10742,7 @@
         </is>
       </c>
       <c r="G303" s="3" t="n">
-        <v>-110.68</v>
+        <v>110.68</v>
       </c>
     </row>
     <row r="304">
@@ -10775,7 +10775,7 @@
         </is>
       </c>
       <c r="G304" s="3" t="n">
-        <v>-157.08</v>
+        <v>157.08</v>
       </c>
     </row>
     <row r="305">
@@ -10808,7 +10808,7 @@
         </is>
       </c>
       <c r="G305" s="3" t="n">
-        <v>-178.82</v>
+        <v>178.82</v>
       </c>
     </row>
     <row r="306">
@@ -10841,7 +10841,7 @@
         </is>
       </c>
       <c r="G306" s="3" t="n">
-        <v>-72.93000000000001</v>
+        <v>72.93000000000001</v>
       </c>
     </row>
     <row r="307">
@@ -10874,7 +10874,7 @@
         </is>
       </c>
       <c r="G307" s="3" t="n">
-        <v>-30.29</v>
+        <v>30.29</v>
       </c>
     </row>
     <row r="308">
@@ -10907,7 +10907,7 @@
         </is>
       </c>
       <c r="G308" s="3" t="n">
-        <v>-1838.55</v>
+        <v>1838.55</v>
       </c>
     </row>
     <row r="309">
@@ -10940,7 +10940,7 @@
         </is>
       </c>
       <c r="G309" s="3" t="n">
-        <v>-157.08</v>
+        <v>157.08</v>
       </c>
     </row>
     <row r="310">
@@ -10973,7 +10973,7 @@
         </is>
       </c>
       <c r="G310" s="3" t="n">
-        <v>-134.07</v>
+        <v>134.07</v>
       </c>
     </row>
     <row r="311">
@@ -11006,7 +11006,7 @@
         </is>
       </c>
       <c r="G311" s="3" t="n">
-        <v>-72.93000000000001</v>
+        <v>72.93000000000001</v>
       </c>
     </row>
     <row r="312">
@@ -11039,7 +11039,7 @@
         </is>
       </c>
       <c r="G312" s="3" t="n">
-        <v>-30.29</v>
+        <v>30.29</v>
       </c>
     </row>
     <row r="313">
@@ -11072,7 +11072,7 @@
         </is>
       </c>
       <c r="G313" s="3" t="n">
-        <v>-1313.25</v>
+        <v>1313.25</v>
       </c>
     </row>
     <row r="314">
@@ -11105,7 +11105,7 @@
         </is>
       </c>
       <c r="G314" s="3" t="n">
-        <v>-251.22</v>
+        <v>251.22</v>
       </c>
     </row>
     <row r="315">
@@ -11138,7 +11138,7 @@
         </is>
       </c>
       <c r="G315" s="3" t="n">
-        <v>-72.93000000000001</v>
+        <v>72.93000000000001</v>
       </c>
     </row>
     <row r="316">
@@ -11171,7 +11171,7 @@
         </is>
       </c>
       <c r="G316" s="3" t="n">
-        <v>-30.29</v>
+        <v>30.29</v>
       </c>
     </row>
     <row r="317">
@@ -11204,7 +11204,7 @@
         </is>
       </c>
       <c r="G317" s="3" t="n">
-        <v>-587.1</v>
+        <v>587.1</v>
       </c>
     </row>
     <row r="318">
@@ -11237,7 +11237,7 @@
         </is>
       </c>
       <c r="G318" s="3" t="n">
-        <v>-2101.2</v>
+        <v>2101.2</v>
       </c>
     </row>
     <row r="319">
@@ -11270,7 +11270,7 @@
         </is>
       </c>
       <c r="G319" s="3" t="n">
-        <v>-157.08</v>
+        <v>157.08</v>
       </c>
     </row>
     <row r="320">
@@ -11303,7 +11303,7 @@
         </is>
       </c>
       <c r="G320" s="3" t="n">
-        <v>-157.08</v>
+        <v>157.08</v>
       </c>
     </row>
     <row r="321">
@@ -11336,7 +11336,7 @@
         </is>
       </c>
       <c r="G321" s="3" t="n">
-        <v>-134.07</v>
+        <v>134.07</v>
       </c>
     </row>
     <row r="322">
@@ -11369,7 +11369,7 @@
         </is>
       </c>
       <c r="G322" s="3" t="n">
-        <v>-72.93000000000001</v>
+        <v>72.93000000000001</v>
       </c>
     </row>
     <row r="323">
@@ -11402,7 +11402,7 @@
         </is>
       </c>
       <c r="G323" s="3" t="n">
-        <v>-30.29</v>
+        <v>30.29</v>
       </c>
     </row>
     <row r="324">
@@ -11435,7 +11435,7 @@
         </is>
       </c>
       <c r="G324" s="3" t="n">
-        <v>-1313.25</v>
+        <v>1313.25</v>
       </c>
     </row>
     <row r="325">

</xml_diff>

<commit_message>
Update web reports - 2025-11-16 08:14:39
</commit_message>
<xml_diff>
--- a/quickbook_summary.xlsx
+++ b/quickbook_summary.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Invoice" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cost" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cost account sum" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -541,7 +542,7 @@
         </is>
       </c>
       <c r="H2" s="4" t="n">
-        <v>200</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3">
@@ -577,7 +578,7 @@
         </is>
       </c>
       <c r="H3" s="4" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
@@ -613,7 +614,7 @@
         </is>
       </c>
       <c r="H4" s="4" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5">
@@ -649,7 +650,7 @@
         </is>
       </c>
       <c r="H5" s="4" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6">
@@ -721,7 +722,7 @@
         </is>
       </c>
       <c r="H7" s="4" t="n">
-        <v>200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="8">
@@ -757,7 +758,7 @@
         </is>
       </c>
       <c r="H8" s="4" t="n">
-        <v>200</v>
+        <v>700</v>
       </c>
     </row>
     <row r="9">
@@ -793,7 +794,7 @@
         </is>
       </c>
       <c r="H9" s="4" t="n">
-        <v>300</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
@@ -829,7 +830,7 @@
         </is>
       </c>
       <c r="H10" s="4" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11">
@@ -865,7 +866,7 @@
         </is>
       </c>
       <c r="H11" s="4" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12">
@@ -901,7 +902,7 @@
         </is>
       </c>
       <c r="H12" s="4" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
     </row>
     <row r="13">
@@ -973,7 +974,7 @@
         </is>
       </c>
       <c r="H14" s="4" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
     </row>
     <row r="15">
@@ -1009,7 +1010,7 @@
         </is>
       </c>
       <c r="H15" s="4" t="n">
-        <v>300</v>
+        <v>700</v>
       </c>
     </row>
     <row r="16">
@@ -1189,7 +1190,7 @@
         </is>
       </c>
       <c r="H20" s="4" t="n">
-        <v>400</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21">
@@ -1225,7 +1226,7 @@
         </is>
       </c>
       <c r="H21" s="4" t="n">
-        <v>400</v>
+        <v>500</v>
       </c>
     </row>
     <row r="22">
@@ -1261,7 +1262,7 @@
         </is>
       </c>
       <c r="H22" s="4" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23">
@@ -1297,7 +1298,7 @@
         </is>
       </c>
       <c r="H23" s="4" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24">
@@ -1369,7 +1370,7 @@
         </is>
       </c>
       <c r="H25" s="4" t="n">
-        <v>400</v>
+        <v>600</v>
       </c>
     </row>
     <row r="26">
@@ -1405,7 +1406,7 @@
         </is>
       </c>
       <c r="H26" s="4" t="n">
-        <v>400</v>
+        <v>700</v>
       </c>
     </row>
     <row r="27">
@@ -1455,7 +1456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H674"/>
+  <dimension ref="A1:H673"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -13547,7 +13548,7 @@
         </is>
       </c>
       <c r="H339" s="4" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="340">
@@ -13583,7 +13584,7 @@
         </is>
       </c>
       <c r="H340" s="4" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="341">
@@ -13619,7 +13620,7 @@
         </is>
       </c>
       <c r="H341" s="4" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="342">
@@ -20528,34 +20529,34 @@
     </row>
     <row r="538">
       <c r="A538" s="2" t="n">
-        <v>45957</v>
+        <v>45958</v>
       </c>
       <c r="B538" s="3" t="inlineStr">
         <is>
-          <t>1100 · Trade Debtors</t>
+          <t>5115 · Rent - Equipment (direct)</t>
         </is>
       </c>
       <c r="C538" s="5" t="n">
-        <v>186293.56</v>
+        <v>2076</v>
       </c>
       <c r="D538" s="3" t="inlineStr">
         <is>
-          <t>Payment</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="E538" s="3" t="inlineStr">
         <is>
-          <t>7224263064</t>
+          <t>254635154-001</t>
         </is>
       </c>
       <c r="F538" s="3" t="inlineStr">
         <is>
-          <t>CIN25-002</t>
+          <t>FORKLIFT VARIABLE REACH 10000# 50'-62'</t>
         </is>
       </c>
       <c r="G538" s="3" t="inlineStr">
         <is>
-          <t>1504 · Undeposited Funds</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="H538" s="4" t="n">
@@ -20572,7 +20573,7 @@
         </is>
       </c>
       <c r="C539" s="5" t="n">
-        <v>2076</v>
+        <v>292.74</v>
       </c>
       <c r="D539" s="3" t="inlineStr">
         <is>
@@ -20586,7 +20587,7 @@
       </c>
       <c r="F539" s="3" t="inlineStr">
         <is>
-          <t>FORKLIFT VARIABLE REACH 10000# 50'-62'</t>
+          <t>Taxes &amp; Fees</t>
         </is>
       </c>
       <c r="G539" s="3" t="inlineStr">
@@ -20608,7 +20609,7 @@
         </is>
       </c>
       <c r="C540" s="5" t="n">
-        <v>292.74</v>
+        <v>540.5</v>
       </c>
       <c r="D540" s="3" t="inlineStr">
         <is>
@@ -20622,7 +20623,7 @@
       </c>
       <c r="F540" s="3" t="inlineStr">
         <is>
-          <t>Taxes &amp; Fees</t>
+          <t>Delivery &amp; Pick Up Charge</t>
         </is>
       </c>
       <c r="G540" s="3" t="inlineStr">
@@ -20636,15 +20637,15 @@
     </row>
     <row r="541">
       <c r="A541" s="2" t="n">
-        <v>45958</v>
+        <v>45959</v>
       </c>
       <c r="B541" s="3" t="inlineStr">
         <is>
-          <t>5115 · Rent - Equipment (direct)</t>
+          <t>5120 · Outside services (Direct)</t>
         </is>
       </c>
       <c r="C541" s="5" t="n">
-        <v>540.5</v>
+        <v>835</v>
       </c>
       <c r="D541" s="3" t="inlineStr">
         <is>
@@ -20653,12 +20654,12 @@
       </c>
       <c r="E541" s="3" t="inlineStr">
         <is>
-          <t>254635154-001</t>
+          <t>2204771</t>
         </is>
       </c>
       <c r="F541" s="3" t="inlineStr">
         <is>
-          <t>Delivery &amp; Pick Up Charge</t>
+          <t>Delivery Hauling</t>
         </is>
       </c>
       <c r="G541" s="3" t="inlineStr">
@@ -20680,7 +20681,7 @@
         </is>
       </c>
       <c r="C542" s="5" t="n">
-        <v>835</v>
+        <v>2500</v>
       </c>
       <c r="D542" s="3" t="inlineStr">
         <is>
@@ -20694,7 +20695,7 @@
       </c>
       <c r="F542" s="3" t="inlineStr">
         <is>
-          <t>Delivery Hauling</t>
+          <t>Hauling Rebillable</t>
         </is>
       </c>
       <c r="G542" s="3" t="inlineStr">
@@ -20716,7 +20717,7 @@
         </is>
       </c>
       <c r="C543" s="5" t="n">
-        <v>2500</v>
+        <v>208.75</v>
       </c>
       <c r="D543" s="3" t="inlineStr">
         <is>
@@ -20730,7 +20731,7 @@
       </c>
       <c r="F543" s="3" t="inlineStr">
         <is>
-          <t>Hauling Rebillable</t>
+          <t>Fuel Charge</t>
         </is>
       </c>
       <c r="G543" s="3" t="inlineStr">
@@ -20752,7 +20753,7 @@
         </is>
       </c>
       <c r="C544" s="5" t="n">
-        <v>208.75</v>
+        <v>65.13</v>
       </c>
       <c r="D544" s="3" t="inlineStr">
         <is>
@@ -20766,7 +20767,7 @@
       </c>
       <c r="F544" s="3" t="inlineStr">
         <is>
-          <t>Fuel Charge</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="G544" s="3" t="inlineStr">
@@ -20780,34 +20781,34 @@
     </row>
     <row r="545">
       <c r="A545" s="2" t="n">
-        <v>45959</v>
+        <v>45960</v>
       </c>
       <c r="B545" s="3" t="inlineStr">
         <is>
-          <t>5120 · Outside services (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C545" s="5" t="n">
-        <v>65.13</v>
+        <v>293.55</v>
       </c>
       <c r="D545" s="3" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>Invoice</t>
         </is>
       </c>
       <c r="E545" s="3" t="inlineStr">
         <is>
-          <t>2204771</t>
+          <t>CIN25-003</t>
         </is>
       </c>
       <c r="F545" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>Badger Hydrovac With Operator - Overtime</t>
         </is>
       </c>
       <c r="G545" s="3" t="inlineStr">
         <is>
-          <t>2000 · Accounts Payable</t>
+          <t>1100 · Trade Debtors</t>
         </is>
       </c>
       <c r="H545" s="4" t="n">
@@ -20928,11 +20929,11 @@
       </c>
       <c r="B549" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5120 · Outside services (Direct)</t>
         </is>
       </c>
       <c r="C549" s="5" t="n">
-        <v>293.55</v>
+        <v>217.18</v>
       </c>
       <c r="D549" s="3" t="inlineStr">
         <is>
@@ -20946,7 +20947,7 @@
       </c>
       <c r="F549" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator - Overtime</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G549" s="3" t="inlineStr">
@@ -20968,7 +20969,7 @@
         </is>
       </c>
       <c r="C550" s="5" t="n">
-        <v>217.18</v>
+        <v>72.93000000000001</v>
       </c>
       <c r="D550" s="3" t="inlineStr">
         <is>
@@ -20982,7 +20983,7 @@
       </c>
       <c r="F550" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G550" s="3" t="inlineStr">
@@ -21004,7 +21005,7 @@
         </is>
       </c>
       <c r="C551" s="5" t="n">
-        <v>72.93000000000001</v>
+        <v>30.29</v>
       </c>
       <c r="D551" s="3" t="inlineStr">
         <is>
@@ -21018,7 +21019,7 @@
       </c>
       <c r="F551" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G551" s="3" t="inlineStr">
@@ -21040,7 +21041,7 @@
         </is>
       </c>
       <c r="C552" s="5" t="n">
-        <v>30.29</v>
+        <v>2101.2</v>
       </c>
       <c r="D552" s="3" t="inlineStr">
         <is>
@@ -21054,7 +21055,7 @@
       </c>
       <c r="F552" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G552" s="3" t="inlineStr">
@@ -21076,7 +21077,7 @@
         </is>
       </c>
       <c r="C553" s="5" t="n">
-        <v>2101.2</v>
+        <v>157.08</v>
       </c>
       <c r="D553" s="3" t="inlineStr">
         <is>
@@ -21090,7 +21091,7 @@
       </c>
       <c r="F553" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G553" s="3" t="inlineStr">
@@ -21112,7 +21113,7 @@
         </is>
       </c>
       <c r="C554" s="5" t="n">
-        <v>157.08</v>
+        <v>217.18</v>
       </c>
       <c r="D554" s="3" t="inlineStr">
         <is>
@@ -21126,7 +21127,7 @@
       </c>
       <c r="F554" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G554" s="3" t="inlineStr">
@@ -21148,7 +21149,7 @@
         </is>
       </c>
       <c r="C555" s="5" t="n">
-        <v>217.18</v>
+        <v>72.93000000000001</v>
       </c>
       <c r="D555" s="3" t="inlineStr">
         <is>
@@ -21162,7 +21163,7 @@
       </c>
       <c r="F555" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G555" s="3" t="inlineStr">
@@ -21184,7 +21185,7 @@
         </is>
       </c>
       <c r="C556" s="5" t="n">
-        <v>72.93000000000001</v>
+        <v>30.29</v>
       </c>
       <c r="D556" s="3" t="inlineStr">
         <is>
@@ -21198,7 +21199,7 @@
       </c>
       <c r="F556" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G556" s="3" t="inlineStr">
@@ -21220,7 +21221,7 @@
         </is>
       </c>
       <c r="C557" s="5" t="n">
-        <v>30.29</v>
+        <v>2101.2</v>
       </c>
       <c r="D557" s="3" t="inlineStr">
         <is>
@@ -21234,7 +21235,7 @@
       </c>
       <c r="F557" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G557" s="3" t="inlineStr">
@@ -21256,7 +21257,7 @@
         </is>
       </c>
       <c r="C558" s="5" t="n">
-        <v>2101.2</v>
+        <v>157.08</v>
       </c>
       <c r="D558" s="3" t="inlineStr">
         <is>
@@ -21270,7 +21271,7 @@
       </c>
       <c r="F558" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G558" s="3" t="inlineStr">
@@ -21292,7 +21293,7 @@
         </is>
       </c>
       <c r="C559" s="5" t="n">
-        <v>157.08</v>
+        <v>217.18</v>
       </c>
       <c r="D559" s="3" t="inlineStr">
         <is>
@@ -21306,7 +21307,7 @@
       </c>
       <c r="F559" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G559" s="3" t="inlineStr">
@@ -21328,7 +21329,7 @@
         </is>
       </c>
       <c r="C560" s="5" t="n">
-        <v>217.18</v>
+        <v>218.79</v>
       </c>
       <c r="D560" s="3" t="inlineStr">
         <is>
@@ -21342,7 +21343,7 @@
       </c>
       <c r="F560" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G560" s="3" t="inlineStr">
@@ -21364,7 +21365,7 @@
         </is>
       </c>
       <c r="C561" s="5" t="n">
-        <v>218.79</v>
+        <v>90.87</v>
       </c>
       <c r="D561" s="3" t="inlineStr">
         <is>
@@ -21378,7 +21379,7 @@
       </c>
       <c r="F561" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G561" s="3" t="inlineStr">
@@ -21400,7 +21401,7 @@
         </is>
       </c>
       <c r="C562" s="5" t="n">
-        <v>90.87</v>
+        <v>6303.6</v>
       </c>
       <c r="D562" s="3" t="inlineStr">
         <is>
@@ -21414,7 +21415,7 @@
       </c>
       <c r="F562" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G562" s="3" t="inlineStr">
@@ -21436,7 +21437,7 @@
         </is>
       </c>
       <c r="C563" s="5" t="n">
-        <v>6303.6</v>
+        <v>471.24</v>
       </c>
       <c r="D563" s="3" t="inlineStr">
         <is>
@@ -21450,7 +21451,7 @@
       </c>
       <c r="F563" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G563" s="3" t="inlineStr">
@@ -21472,7 +21473,7 @@
         </is>
       </c>
       <c r="C564" s="5" t="n">
-        <v>471.24</v>
+        <v>440.33</v>
       </c>
       <c r="D564" s="3" t="inlineStr">
         <is>
@@ -21486,7 +21487,7 @@
       </c>
       <c r="F564" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Badger Hydrovac With Operator - Overtime</t>
         </is>
       </c>
       <c r="G564" s="3" t="inlineStr">
@@ -21508,7 +21509,7 @@
         </is>
       </c>
       <c r="C565" s="5" t="n">
-        <v>440.33</v>
+        <v>398.35</v>
       </c>
       <c r="D565" s="3" t="inlineStr">
         <is>
@@ -21522,7 +21523,7 @@
       </c>
       <c r="F565" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator - Overtime</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G565" s="3" t="inlineStr">
@@ -21544,7 +21545,7 @@
         </is>
       </c>
       <c r="C566" s="5" t="n">
-        <v>398.35</v>
+        <v>193.17</v>
       </c>
       <c r="D566" s="3" t="inlineStr">
         <is>
@@ -21580,7 +21581,7 @@
         </is>
       </c>
       <c r="C567" s="5" t="n">
-        <v>193.17</v>
+        <v>72.93000000000001</v>
       </c>
       <c r="D567" s="3" t="inlineStr">
         <is>
@@ -21594,7 +21595,7 @@
       </c>
       <c r="F567" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G567" s="3" t="inlineStr">
@@ -21616,7 +21617,7 @@
         </is>
       </c>
       <c r="C568" s="5" t="n">
-        <v>72.93000000000001</v>
+        <v>30.29</v>
       </c>
       <c r="D568" s="3" t="inlineStr">
         <is>
@@ -21630,7 +21631,7 @@
       </c>
       <c r="F568" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G568" s="3" t="inlineStr">
@@ -21652,7 +21653,7 @@
         </is>
       </c>
       <c r="C569" s="5" t="n">
-        <v>30.29</v>
+        <v>2101.2</v>
       </c>
       <c r="D569" s="3" t="inlineStr">
         <is>
@@ -21666,7 +21667,7 @@
       </c>
       <c r="F569" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G569" s="3" t="inlineStr">
@@ -21688,7 +21689,7 @@
         </is>
       </c>
       <c r="C570" s="5" t="n">
-        <v>2101.2</v>
+        <v>157.08</v>
       </c>
       <c r="D570" s="3" t="inlineStr">
         <is>
@@ -21702,7 +21703,7 @@
       </c>
       <c r="F570" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G570" s="3" t="inlineStr">
@@ -21724,7 +21725,7 @@
         </is>
       </c>
       <c r="C571" s="5" t="n">
-        <v>157.08</v>
+        <v>205.18</v>
       </c>
       <c r="D571" s="3" t="inlineStr">
         <is>
@@ -21738,7 +21739,7 @@
       </c>
       <c r="F571" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G571" s="3" t="inlineStr">
@@ -21760,7 +21761,7 @@
         </is>
       </c>
       <c r="C572" s="5" t="n">
-        <v>205.18</v>
+        <v>72.93000000000001</v>
       </c>
       <c r="D572" s="3" t="inlineStr">
         <is>
@@ -21774,7 +21775,7 @@
       </c>
       <c r="F572" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G572" s="3" t="inlineStr">
@@ -21796,7 +21797,7 @@
         </is>
       </c>
       <c r="C573" s="5" t="n">
-        <v>72.93000000000001</v>
+        <v>30.29</v>
       </c>
       <c r="D573" s="3" t="inlineStr">
         <is>
@@ -21810,7 +21811,7 @@
       </c>
       <c r="F573" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G573" s="3" t="inlineStr">
@@ -21832,7 +21833,7 @@
         </is>
       </c>
       <c r="C574" s="5" t="n">
-        <v>30.29</v>
+        <v>2101.2</v>
       </c>
       <c r="D574" s="3" t="inlineStr">
         <is>
@@ -21846,7 +21847,7 @@
       </c>
       <c r="F574" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G574" s="3" t="inlineStr">
@@ -21868,7 +21869,7 @@
         </is>
       </c>
       <c r="C575" s="5" t="n">
-        <v>2101.2</v>
+        <v>157.08</v>
       </c>
       <c r="D575" s="3" t="inlineStr">
         <is>
@@ -21882,7 +21883,7 @@
       </c>
       <c r="F575" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G575" s="3" t="inlineStr">
@@ -21904,7 +21905,7 @@
         </is>
       </c>
       <c r="C576" s="5" t="n">
-        <v>157.08</v>
+        <v>146.78</v>
       </c>
       <c r="D576" s="3" t="inlineStr">
         <is>
@@ -21918,7 +21919,7 @@
       </c>
       <c r="F576" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G576" s="3" t="inlineStr">
@@ -21940,7 +21941,7 @@
         </is>
       </c>
       <c r="C577" s="5" t="n">
-        <v>146.78</v>
+        <v>157.08</v>
       </c>
       <c r="D577" s="3" t="inlineStr">
         <is>
@@ -21954,7 +21955,7 @@
       </c>
       <c r="F577" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G577" s="3" t="inlineStr">
@@ -21976,7 +21977,7 @@
         </is>
       </c>
       <c r="C578" s="5" t="n">
-        <v>157.08</v>
+        <v>160.94</v>
       </c>
       <c r="D578" s="3" t="inlineStr">
         <is>
@@ -21990,7 +21991,7 @@
       </c>
       <c r="F578" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G578" s="3" t="inlineStr">
@@ -22012,7 +22013,7 @@
         </is>
       </c>
       <c r="C579" s="5" t="n">
-        <v>160.94</v>
+        <v>72.93000000000001</v>
       </c>
       <c r="D579" s="3" t="inlineStr">
         <is>
@@ -22026,7 +22027,7 @@
       </c>
       <c r="F579" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G579" s="3" t="inlineStr">
@@ -22048,7 +22049,7 @@
         </is>
       </c>
       <c r="C580" s="5" t="n">
-        <v>72.93000000000001</v>
+        <v>30.29</v>
       </c>
       <c r="D580" s="3" t="inlineStr">
         <is>
@@ -22062,7 +22063,7 @@
       </c>
       <c r="F580" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G580" s="3" t="inlineStr">
@@ -22084,7 +22085,7 @@
         </is>
       </c>
       <c r="C581" s="5" t="n">
-        <v>30.29</v>
+        <v>1707.23</v>
       </c>
       <c r="D581" s="3" t="inlineStr">
         <is>
@@ -22098,7 +22099,7 @@
       </c>
       <c r="F581" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G581" s="3" t="inlineStr">
@@ -22120,7 +22121,7 @@
         </is>
       </c>
       <c r="C582" s="5" t="n">
-        <v>1707.23</v>
+        <v>217.18</v>
       </c>
       <c r="D582" s="3" t="inlineStr">
         <is>
@@ -22134,7 +22135,7 @@
       </c>
       <c r="F582" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G582" s="3" t="inlineStr">
@@ -22156,7 +22157,7 @@
         </is>
       </c>
       <c r="C583" s="5" t="n">
-        <v>217.18</v>
+        <v>72.93000000000001</v>
       </c>
       <c r="D583" s="3" t="inlineStr">
         <is>
@@ -22170,7 +22171,7 @@
       </c>
       <c r="F583" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G583" s="3" t="inlineStr">
@@ -22192,7 +22193,7 @@
         </is>
       </c>
       <c r="C584" s="5" t="n">
-        <v>72.93000000000001</v>
+        <v>30.29</v>
       </c>
       <c r="D584" s="3" t="inlineStr">
         <is>
@@ -22206,7 +22207,7 @@
       </c>
       <c r="F584" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G584" s="3" t="inlineStr">
@@ -22228,7 +22229,7 @@
         </is>
       </c>
       <c r="C585" s="5" t="n">
-        <v>30.29</v>
+        <v>2101.2</v>
       </c>
       <c r="D585" s="3" t="inlineStr">
         <is>
@@ -22242,7 +22243,7 @@
       </c>
       <c r="F585" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G585" s="3" t="inlineStr">
@@ -22264,7 +22265,7 @@
         </is>
       </c>
       <c r="C586" s="5" t="n">
-        <v>2101.2</v>
+        <v>157.08</v>
       </c>
       <c r="D586" s="3" t="inlineStr">
         <is>
@@ -22278,7 +22279,7 @@
       </c>
       <c r="F586" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G586" s="3" t="inlineStr">
@@ -22300,7 +22301,7 @@
         </is>
       </c>
       <c r="C587" s="5" t="n">
-        <v>157.08</v>
+        <v>201.2</v>
       </c>
       <c r="D587" s="3" t="inlineStr">
         <is>
@@ -22314,7 +22315,7 @@
       </c>
       <c r="F587" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G587" s="3" t="inlineStr">
@@ -22336,7 +22337,7 @@
         </is>
       </c>
       <c r="C588" s="5" t="n">
-        <v>201.2</v>
+        <v>72.93000000000001</v>
       </c>
       <c r="D588" s="3" t="inlineStr">
         <is>
@@ -22350,7 +22351,7 @@
       </c>
       <c r="F588" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G588" s="3" t="inlineStr">
@@ -22372,7 +22373,7 @@
         </is>
       </c>
       <c r="C589" s="5" t="n">
-        <v>72.93000000000001</v>
+        <v>30.29</v>
       </c>
       <c r="D589" s="3" t="inlineStr">
         <is>
@@ -22386,7 +22387,7 @@
       </c>
       <c r="F589" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G589" s="3" t="inlineStr">
@@ -22408,7 +22409,7 @@
         </is>
       </c>
       <c r="C590" s="5" t="n">
-        <v>30.29</v>
+        <v>2101.2</v>
       </c>
       <c r="D590" s="3" t="inlineStr">
         <is>
@@ -22422,7 +22423,7 @@
       </c>
       <c r="F590" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G590" s="3" t="inlineStr">
@@ -22444,7 +22445,7 @@
         </is>
       </c>
       <c r="C591" s="5" t="n">
-        <v>2101.2</v>
+        <v>157.08</v>
       </c>
       <c r="D591" s="3" t="inlineStr">
         <is>
@@ -22458,7 +22459,7 @@
       </c>
       <c r="F591" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G591" s="3" t="inlineStr">
@@ -22480,7 +22481,7 @@
         </is>
       </c>
       <c r="C592" s="5" t="n">
-        <v>157.08</v>
+        <v>217.18</v>
       </c>
       <c r="D592" s="3" t="inlineStr">
         <is>
@@ -22494,7 +22495,7 @@
       </c>
       <c r="F592" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G592" s="3" t="inlineStr">
@@ -22516,7 +22517,7 @@
         </is>
       </c>
       <c r="C593" s="5" t="n">
-        <v>217.18</v>
+        <v>72.93000000000001</v>
       </c>
       <c r="D593" s="3" t="inlineStr">
         <is>
@@ -22530,7 +22531,7 @@
       </c>
       <c r="F593" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G593" s="3" t="inlineStr">
@@ -22552,7 +22553,7 @@
         </is>
       </c>
       <c r="C594" s="5" t="n">
-        <v>72.93000000000001</v>
+        <v>30.29</v>
       </c>
       <c r="D594" s="3" t="inlineStr">
         <is>
@@ -22566,7 +22567,7 @@
       </c>
       <c r="F594" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G594" s="3" t="inlineStr">
@@ -22588,7 +22589,7 @@
         </is>
       </c>
       <c r="C595" s="5" t="n">
-        <v>30.29</v>
+        <v>2101.2</v>
       </c>
       <c r="D595" s="3" t="inlineStr">
         <is>
@@ -22602,7 +22603,7 @@
       </c>
       <c r="F595" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G595" s="3" t="inlineStr">
@@ -22624,7 +22625,7 @@
         </is>
       </c>
       <c r="C596" s="5" t="n">
-        <v>2101.2</v>
+        <v>157.08</v>
       </c>
       <c r="D596" s="3" t="inlineStr">
         <is>
@@ -22638,7 +22639,7 @@
       </c>
       <c r="F596" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G596" s="3" t="inlineStr">
@@ -22660,7 +22661,7 @@
         </is>
       </c>
       <c r="C597" s="5" t="n">
-        <v>157.08</v>
+        <v>364.86</v>
       </c>
       <c r="D597" s="3" t="inlineStr">
         <is>
@@ -22674,7 +22675,7 @@
       </c>
       <c r="F597" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G597" s="3" t="inlineStr">
@@ -22696,7 +22697,7 @@
         </is>
       </c>
       <c r="C598" s="5" t="n">
-        <v>364.86</v>
+        <v>145.86</v>
       </c>
       <c r="D598" s="3" t="inlineStr">
         <is>
@@ -22710,7 +22711,7 @@
       </c>
       <c r="F598" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G598" s="3" t="inlineStr">
@@ -22732,7 +22733,7 @@
         </is>
       </c>
       <c r="C599" s="5" t="n">
-        <v>145.86</v>
+        <v>60.58</v>
       </c>
       <c r="D599" s="3" t="inlineStr">
         <is>
@@ -22746,7 +22747,7 @@
       </c>
       <c r="F599" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G599" s="3" t="inlineStr">
@@ -22768,7 +22769,7 @@
         </is>
       </c>
       <c r="C600" s="5" t="n">
-        <v>60.58</v>
+        <v>3939.75</v>
       </c>
       <c r="D600" s="3" t="inlineStr">
         <is>
@@ -22782,7 +22783,7 @@
       </c>
       <c r="F600" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G600" s="3" t="inlineStr">
@@ -22804,7 +22805,7 @@
         </is>
       </c>
       <c r="C601" s="5" t="n">
-        <v>3939.75</v>
+        <v>314.16</v>
       </c>
       <c r="D601" s="3" t="inlineStr">
         <is>
@@ -22818,7 +22819,7 @@
       </c>
       <c r="F601" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G601" s="3" t="inlineStr">
@@ -22840,7 +22841,7 @@
         </is>
       </c>
       <c r="C602" s="5" t="n">
-        <v>314.16</v>
+        <v>418.89</v>
       </c>
       <c r="D602" s="3" t="inlineStr">
         <is>
@@ -22854,7 +22855,7 @@
       </c>
       <c r="F602" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G602" s="3" t="inlineStr">
@@ -22876,7 +22877,7 @@
         </is>
       </c>
       <c r="C603" s="5" t="n">
-        <v>418.89</v>
+        <v>145.86</v>
       </c>
       <c r="D603" s="3" t="inlineStr">
         <is>
@@ -22890,7 +22891,7 @@
       </c>
       <c r="F603" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G603" s="3" t="inlineStr">
@@ -22912,7 +22913,7 @@
         </is>
       </c>
       <c r="C604" s="5" t="n">
-        <v>145.86</v>
+        <v>60.58</v>
       </c>
       <c r="D604" s="3" t="inlineStr">
         <is>
@@ -22926,7 +22927,7 @@
       </c>
       <c r="F604" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G604" s="3" t="inlineStr">
@@ -22948,7 +22949,7 @@
         </is>
       </c>
       <c r="C605" s="5" t="n">
-        <v>60.58</v>
+        <v>293.56</v>
       </c>
       <c r="D605" s="3" t="inlineStr">
         <is>
@@ -22962,7 +22963,7 @@
       </c>
       <c r="F605" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator Overtime</t>
         </is>
       </c>
       <c r="G605" s="3" t="inlineStr">
@@ -22984,7 +22985,7 @@
         </is>
       </c>
       <c r="C606" s="5" t="n">
-        <v>293.56</v>
+        <v>4202.4</v>
       </c>
       <c r="D606" s="3" t="inlineStr">
         <is>
@@ -22998,7 +22999,7 @@
       </c>
       <c r="F606" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator Overtime</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G606" s="3" t="inlineStr">
@@ -23020,7 +23021,7 @@
         </is>
       </c>
       <c r="C607" s="5" t="n">
-        <v>4202.4</v>
+        <v>314.16</v>
       </c>
       <c r="D607" s="3" t="inlineStr">
         <is>
@@ -23034,7 +23035,7 @@
       </c>
       <c r="F607" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G607" s="3" t="inlineStr">
@@ -23056,7 +23057,7 @@
         </is>
       </c>
       <c r="C608" s="5" t="n">
-        <v>314.16</v>
+        <v>447.33</v>
       </c>
       <c r="D608" s="3" t="inlineStr">
         <is>
@@ -23070,7 +23071,7 @@
       </c>
       <c r="F608" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G608" s="3" t="inlineStr">
@@ -23092,7 +23093,7 @@
         </is>
       </c>
       <c r="C609" s="5" t="n">
-        <v>447.33</v>
+        <v>145.86</v>
       </c>
       <c r="D609" s="3" t="inlineStr">
         <is>
@@ -23106,7 +23107,7 @@
       </c>
       <c r="F609" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G609" s="3" t="inlineStr">
@@ -23128,7 +23129,7 @@
         </is>
       </c>
       <c r="C610" s="5" t="n">
-        <v>145.86</v>
+        <v>60.58</v>
       </c>
       <c r="D610" s="3" t="inlineStr">
         <is>
@@ -23142,7 +23143,7 @@
       </c>
       <c r="F610" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G610" s="3" t="inlineStr">
@@ -23164,7 +23165,7 @@
         </is>
       </c>
       <c r="C611" s="5" t="n">
-        <v>60.58</v>
+        <v>440.33</v>
       </c>
       <c r="D611" s="3" t="inlineStr">
         <is>
@@ -23178,7 +23179,7 @@
       </c>
       <c r="F611" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator Overtime</t>
         </is>
       </c>
       <c r="G611" s="3" t="inlineStr">
@@ -23200,7 +23201,7 @@
         </is>
       </c>
       <c r="C612" s="5" t="n">
-        <v>440.33</v>
+        <v>4202.4</v>
       </c>
       <c r="D612" s="3" t="inlineStr">
         <is>
@@ -23214,7 +23215,7 @@
       </c>
       <c r="F612" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator Overtime</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G612" s="3" t="inlineStr">
@@ -23236,7 +23237,7 @@
         </is>
       </c>
       <c r="C613" s="5" t="n">
-        <v>4202.4</v>
+        <v>314.16</v>
       </c>
       <c r="D613" s="3" t="inlineStr">
         <is>
@@ -23250,7 +23251,7 @@
       </c>
       <c r="F613" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G613" s="3" t="inlineStr">
@@ -23272,7 +23273,7 @@
         </is>
       </c>
       <c r="C614" s="5" t="n">
-        <v>314.16</v>
+        <v>87</v>
       </c>
       <c r="D614" s="3" t="inlineStr">
         <is>
@@ -23286,7 +23287,7 @@
       </c>
       <c r="F614" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Remote Hose</t>
         </is>
       </c>
       <c r="G614" s="3" t="inlineStr">
@@ -23308,7 +23309,7 @@
         </is>
       </c>
       <c r="C615" s="5" t="n">
-        <v>87</v>
+        <v>952.09</v>
       </c>
       <c r="D615" s="3" t="inlineStr">
         <is>
@@ -23322,7 +23323,7 @@
       </c>
       <c r="F615" s="3" t="inlineStr">
         <is>
-          <t>Remote Hose</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G615" s="3" t="inlineStr">
@@ -23344,7 +23345,7 @@
         </is>
       </c>
       <c r="C616" s="5" t="n">
-        <v>952.09</v>
+        <v>291.72</v>
       </c>
       <c r="D616" s="3" t="inlineStr">
         <is>
@@ -23358,7 +23359,7 @@
       </c>
       <c r="F616" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G616" s="3" t="inlineStr">
@@ -23380,7 +23381,7 @@
         </is>
       </c>
       <c r="C617" s="5" t="n">
-        <v>291.72</v>
+        <v>121.16</v>
       </c>
       <c r="D617" s="3" t="inlineStr">
         <is>
@@ -23394,7 +23395,7 @@
       </c>
       <c r="F617" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G617" s="3" t="inlineStr">
@@ -23416,7 +23417,7 @@
         </is>
       </c>
       <c r="C618" s="5" t="n">
-        <v>121.16</v>
+        <v>1467.76</v>
       </c>
       <c r="D618" s="3" t="inlineStr">
         <is>
@@ -23430,7 +23431,7 @@
       </c>
       <c r="F618" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator Overtime</t>
         </is>
       </c>
       <c r="G618" s="3" t="inlineStr">
@@ -23452,7 +23453,7 @@
         </is>
       </c>
       <c r="C619" s="5" t="n">
-        <v>1467.76</v>
+        <v>8404.799999999999</v>
       </c>
       <c r="D619" s="3" t="inlineStr">
         <is>
@@ -23466,7 +23467,7 @@
       </c>
       <c r="F619" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator Overtime</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G619" s="3" t="inlineStr">
@@ -23488,7 +23489,7 @@
         </is>
       </c>
       <c r="C620" s="5" t="n">
-        <v>8404.799999999999</v>
+        <v>628.3200000000001</v>
       </c>
       <c r="D620" s="3" t="inlineStr">
         <is>
@@ -23502,7 +23503,7 @@
       </c>
       <c r="F620" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G620" s="3" t="inlineStr">
@@ -23524,7 +23525,7 @@
         </is>
       </c>
       <c r="C621" s="5" t="n">
-        <v>628.3200000000001</v>
+        <v>261</v>
       </c>
       <c r="D621" s="3" t="inlineStr">
         <is>
@@ -23538,7 +23539,7 @@
       </c>
       <c r="F621" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Remote Hose</t>
         </is>
       </c>
       <c r="G621" s="3" t="inlineStr">
@@ -23560,7 +23561,7 @@
         </is>
       </c>
       <c r="C622" s="5" t="n">
-        <v>261</v>
+        <v>402.33</v>
       </c>
       <c r="D622" s="3" t="inlineStr">
         <is>
@@ -23574,7 +23575,7 @@
       </c>
       <c r="F622" s="3" t="inlineStr">
         <is>
-          <t>Remote Hose</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G622" s="3" t="inlineStr">
@@ -23596,7 +23597,7 @@
         </is>
       </c>
       <c r="C623" s="5" t="n">
-        <v>402.33</v>
+        <v>145.86</v>
       </c>
       <c r="D623" s="3" t="inlineStr">
         <is>
@@ -23610,7 +23611,7 @@
       </c>
       <c r="F623" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G623" s="3" t="inlineStr">
@@ -23632,7 +23633,7 @@
         </is>
       </c>
       <c r="C624" s="5" t="n">
-        <v>145.86</v>
+        <v>60.58</v>
       </c>
       <c r="D624" s="3" t="inlineStr">
         <is>
@@ -23646,7 +23647,7 @@
       </c>
       <c r="F624" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G624" s="3" t="inlineStr">
@@ -23667,8 +23668,8 @@
           <t>5120 · Outside services (Direct)</t>
         </is>
       </c>
-      <c r="C625" s="5" t="n">
-        <v>60.58</v>
+      <c r="C625" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="D625" s="3" t="inlineStr">
         <is>
@@ -23682,7 +23683,7 @@
       </c>
       <c r="F625" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator Overtime</t>
         </is>
       </c>
       <c r="G625" s="3" t="inlineStr">
@@ -23703,8 +23704,8 @@
           <t>5120 · Outside services (Direct)</t>
         </is>
       </c>
-      <c r="C626" s="3" t="n">
-        <v>0</v>
+      <c r="C626" s="5" t="n">
+        <v>4071.08</v>
       </c>
       <c r="D626" s="3" t="inlineStr">
         <is>
@@ -23718,7 +23719,7 @@
       </c>
       <c r="F626" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator Overtime</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G626" s="3" t="inlineStr">
@@ -23740,7 +23741,7 @@
         </is>
       </c>
       <c r="C627" s="5" t="n">
-        <v>4071.08</v>
+        <v>314.16</v>
       </c>
       <c r="D627" s="3" t="inlineStr">
         <is>
@@ -23754,7 +23755,7 @@
       </c>
       <c r="F627" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G627" s="3" t="inlineStr">
@@ -23776,7 +23777,7 @@
         </is>
       </c>
       <c r="C628" s="5" t="n">
-        <v>314.16</v>
+        <v>130.5</v>
       </c>
       <c r="D628" s="3" t="inlineStr">
         <is>
@@ -23790,7 +23791,7 @@
       </c>
       <c r="F628" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Remote Hose</t>
         </is>
       </c>
       <c r="G628" s="3" t="inlineStr">
@@ -23812,7 +23813,7 @@
         </is>
       </c>
       <c r="C629" s="5" t="n">
-        <v>130.5</v>
+        <v>111.69</v>
       </c>
       <c r="D629" s="3" t="inlineStr">
         <is>
@@ -23826,7 +23827,7 @@
       </c>
       <c r="F629" s="3" t="inlineStr">
         <is>
-          <t>Remote Hose</t>
+          <t>Fluctuating Fuel Recovery</t>
         </is>
       </c>
       <c r="G629" s="3" t="inlineStr">
@@ -23848,7 +23849,7 @@
         </is>
       </c>
       <c r="C630" s="5" t="n">
-        <v>111.69</v>
+        <v>72.93000000000001</v>
       </c>
       <c r="D630" s="3" t="inlineStr">
         <is>
@@ -23862,7 +23863,7 @@
       </c>
       <c r="F630" s="3" t="inlineStr">
         <is>
-          <t>Fluctuating Fuel Recovery</t>
+          <t>Supply Water</t>
         </is>
       </c>
       <c r="G630" s="3" t="inlineStr">
@@ -23884,7 +23885,7 @@
         </is>
       </c>
       <c r="C631" s="5" t="n">
-        <v>72.93000000000001</v>
+        <v>30.29</v>
       </c>
       <c r="D631" s="3" t="inlineStr">
         <is>
@@ -23898,7 +23899,7 @@
       </c>
       <c r="F631" s="3" t="inlineStr">
         <is>
-          <t>Supply Water</t>
+          <t>Consumable Materials</t>
         </is>
       </c>
       <c r="G631" s="3" t="inlineStr">
@@ -23919,8 +23920,8 @@
           <t>5120 · Outside services (Direct)</t>
         </is>
       </c>
-      <c r="C632" s="5" t="n">
-        <v>30.29</v>
+      <c r="C632" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="D632" s="3" t="inlineStr">
         <is>
@@ -23934,7 +23935,7 @@
       </c>
       <c r="F632" s="3" t="inlineStr">
         <is>
-          <t>Consumable Materials</t>
+          <t>Badger Hydrovac With Operator Overtime</t>
         </is>
       </c>
       <c r="G632" s="3" t="inlineStr">
@@ -23955,8 +23956,8 @@
           <t>5120 · Outside services (Direct)</t>
         </is>
       </c>
-      <c r="C633" s="3" t="n">
-        <v>0</v>
+      <c r="C633" s="5" t="n">
+        <v>1050.6</v>
       </c>
       <c r="D633" s="3" t="inlineStr">
         <is>
@@ -23970,7 +23971,7 @@
       </c>
       <c r="F633" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator Overtime</t>
+          <t>Badger Hydrovac With Operator</t>
         </is>
       </c>
       <c r="G633" s="3" t="inlineStr">
@@ -23992,7 +23993,7 @@
         </is>
       </c>
       <c r="C634" s="5" t="n">
-        <v>1050.6</v>
+        <v>157.08</v>
       </c>
       <c r="D634" s="3" t="inlineStr">
         <is>
@@ -24006,7 +24007,7 @@
       </c>
       <c r="F634" s="3" t="inlineStr">
         <is>
-          <t>Badger Hydrovac With Operator</t>
+          <t>Disposition</t>
         </is>
       </c>
       <c r="G634" s="3" t="inlineStr">
@@ -24020,34 +24021,34 @@
     </row>
     <row r="635">
       <c r="A635" s="2" t="n">
-        <v>45960</v>
+        <v>45961</v>
       </c>
       <c r="B635" s="3" t="inlineStr">
         <is>
-          <t>5120 · Outside services (Direct)</t>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
         </is>
       </c>
       <c r="C635" s="5" t="n">
-        <v>157.08</v>
+        <v>350</v>
       </c>
       <c r="D635" s="3" t="inlineStr">
         <is>
-          <t>Invoice</t>
+          <t>General Journal</t>
         </is>
       </c>
       <c r="E635" s="3" t="inlineStr">
         <is>
-          <t>CIN25-003</t>
+          <t>16783</t>
         </is>
       </c>
       <c r="F635" s="3" t="inlineStr">
         <is>
-          <t>Disposition</t>
+          <t>Andy Remillard Per diem for week of 11/03/2025 - 11/09/2025</t>
         </is>
       </c>
       <c r="G635" s="3" t="inlineStr">
         <is>
-          <t>1100 · Trade Debtors</t>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
         </is>
       </c>
       <c r="H635" s="4" t="n">
@@ -24064,7 +24065,7 @@
         </is>
       </c>
       <c r="C636" s="5" t="n">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D636" s="3" t="inlineStr">
         <is>
@@ -24078,7 +24079,7 @@
       </c>
       <c r="F636" s="3" t="inlineStr">
         <is>
-          <t>Andy Remillard Per diem for week of 11/03/2025 - 11/09/2025</t>
+          <t>Brian Krumbholz Per diem for week of 11/03/2025 - 11/09/2025</t>
         </is>
       </c>
       <c r="G636" s="3" t="inlineStr">
@@ -24100,7 +24101,7 @@
         </is>
       </c>
       <c r="C637" s="5" t="n">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="D637" s="3" t="inlineStr">
         <is>
@@ -24114,7 +24115,7 @@
       </c>
       <c r="F637" s="3" t="inlineStr">
         <is>
-          <t>Brian Krumbholz Per diem for week of 11/03/2025 - 11/09/2025</t>
+          <t>Mike Cogswell Per diem for week of 11/03/2025 - 11/09/2025</t>
         </is>
       </c>
       <c r="G637" s="3" t="inlineStr">
@@ -24128,34 +24129,34 @@
     </row>
     <row r="638">
       <c r="A638" s="2" t="n">
-        <v>45961</v>
+        <v>45964</v>
       </c>
       <c r="B638" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>1504 · Undeposited Funds</t>
         </is>
       </c>
       <c r="C638" s="5" t="n">
-        <v>350</v>
+        <v>186293.56</v>
       </c>
       <c r="D638" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Deposit</t>
         </is>
       </c>
       <c r="E638" s="3" t="inlineStr">
         <is>
-          <t>16783</t>
+          <t>7224263064</t>
         </is>
       </c>
       <c r="F638" s="3" t="inlineStr">
         <is>
-          <t>Mike Cogswell Per diem for week of 11/03/2025 - 11/09/2025</t>
+          <t>CIN25-002</t>
         </is>
       </c>
       <c r="G638" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>1006.1 · (NEW) Calif B &amp; T Checking</t>
         </is>
       </c>
       <c r="H638" s="4" t="n">
@@ -24164,34 +24165,34 @@
     </row>
     <row r="639">
       <c r="A639" s="2" t="n">
-        <v>45964</v>
+        <v>45967</v>
       </c>
       <c r="B639" s="3" t="inlineStr">
         <is>
-          <t>1504 · Undeposited Funds</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C639" s="5" t="n">
-        <v>186293.56</v>
+        <v>492.3</v>
       </c>
       <c r="D639" s="3" t="inlineStr">
         <is>
-          <t>Deposit</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="E639" s="3" t="inlineStr">
         <is>
-          <t>7224263064</t>
+          <t>54967992</t>
         </is>
       </c>
       <c r="F639" s="3" t="inlineStr">
         <is>
-          <t>CIN25-002</t>
+          <t xml:space="preserve">	316 Stainless Steel Check Valve with Fluoroelastomer Piston with Rubber Spring-Loaded Piston, 1...</t>
         </is>
       </c>
       <c r="G639" s="3" t="inlineStr">
         <is>
-          <t>1006.1 · (NEW) Calif B &amp; T Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="H639" s="4" t="n">
@@ -24208,7 +24209,7 @@
         </is>
       </c>
       <c r="C640" s="5" t="n">
-        <v>492.3</v>
+        <v>44.9</v>
       </c>
       <c r="D640" s="3" t="inlineStr">
         <is>
@@ -24222,7 +24223,7 @@
       </c>
       <c r="F640" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">	316 Stainless Steel Check Valve with Fluoroelastomer Piston with Rubber Spring-Loaded Piston, 1...</t>
+          <t xml:space="preserve">	UV-Rst Hard Clear FEP Tubing for Chemicals 7/16" ID, 1/2" OD, 10 ft. Length</t>
         </is>
       </c>
       <c r="G640" s="3" t="inlineStr">
@@ -24244,7 +24245,7 @@
         </is>
       </c>
       <c r="C641" s="5" t="n">
-        <v>44.9</v>
+        <v>38.39</v>
       </c>
       <c r="D641" s="3" t="inlineStr">
         <is>
@@ -24258,7 +24259,7 @@
       </c>
       <c r="F641" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">	UV-Rst Hard Clear FEP Tubing for Chemicals 7/16" ID, 1/2" OD, 10 ft. Length</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="G641" s="3" t="inlineStr">
@@ -24280,7 +24281,7 @@
         </is>
       </c>
       <c r="C642" s="5" t="n">
-        <v>38.39</v>
+        <v>11.29</v>
       </c>
       <c r="D642" s="3" t="inlineStr">
         <is>
@@ -24294,7 +24295,7 @@
       </c>
       <c r="F642" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>Shippig</t>
         </is>
       </c>
       <c r="G642" s="3" t="inlineStr">
@@ -24316,7 +24317,7 @@
         </is>
       </c>
       <c r="C643" s="5" t="n">
-        <v>11.29</v>
+        <v>30.42</v>
       </c>
       <c r="D643" s="3" t="inlineStr">
         <is>
@@ -24325,12 +24326,12 @@
       </c>
       <c r="E643" s="3" t="inlineStr">
         <is>
-          <t>54967992</t>
+          <t>54957597</t>
         </is>
       </c>
       <c r="F643" s="3" t="inlineStr">
         <is>
-          <t>Shippig</t>
+          <t xml:space="preserve">	Tapping and Threading Lubricant, Ridgid Nu-Clear, 1 Gallon Jug</t>
         </is>
       </c>
       <c r="G643" s="3" t="inlineStr">
@@ -24352,7 +24353,7 @@
         </is>
       </c>
       <c r="C644" s="5" t="n">
-        <v>30.42</v>
+        <v>1.67</v>
       </c>
       <c r="D644" s="3" t="inlineStr">
         <is>
@@ -24366,7 +24367,7 @@
       </c>
       <c r="F644" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">	Tapping and Threading Lubricant, Ridgid Nu-Clear, 1 Gallon Jug</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="G644" s="3" t="inlineStr">
@@ -24384,11 +24385,11 @@
       </c>
       <c r="B645" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5121 · Freight &amp; Shipping (Direct)</t>
         </is>
       </c>
       <c r="C645" s="5" t="n">
-        <v>1.67</v>
+        <v>16.02</v>
       </c>
       <c r="D645" s="3" t="inlineStr">
         <is>
@@ -24402,7 +24403,7 @@
       </c>
       <c r="F645" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>Shipping &amp; Handling</t>
         </is>
       </c>
       <c r="G645" s="3" t="inlineStr">
@@ -24416,34 +24417,34 @@
     </row>
     <row r="646">
       <c r="A646" s="2" t="n">
-        <v>45967</v>
+        <v>45968</v>
       </c>
       <c r="B646" s="3" t="inlineStr">
         <is>
-          <t>5121 · Freight &amp; Shipping (Direct)</t>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
         </is>
       </c>
       <c r="C646" s="5" t="n">
-        <v>16.02</v>
+        <v>350</v>
       </c>
       <c r="D646" s="3" t="inlineStr">
         <is>
-          <t>Bill</t>
+          <t>General Journal</t>
         </is>
       </c>
       <c r="E646" s="3" t="inlineStr">
         <is>
-          <t>54957597</t>
+          <t>16784</t>
         </is>
       </c>
       <c r="F646" s="3" t="inlineStr">
         <is>
-          <t>Shipping &amp; Handling</t>
+          <t>Andy Remillard Per diem for week of 11/10/2025 - 11/16/2025</t>
         </is>
       </c>
       <c r="G646" s="3" t="inlineStr">
         <is>
-          <t>2000 · Accounts Payable</t>
+          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
         </is>
       </c>
       <c r="H646" s="4" t="n">
@@ -24460,7 +24461,7 @@
         </is>
       </c>
       <c r="C647" s="5" t="n">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="D647" s="3" t="inlineStr">
         <is>
@@ -24474,7 +24475,7 @@
       </c>
       <c r="F647" s="3" t="inlineStr">
         <is>
-          <t>Andy Remillard Per diem for week of 11/10/2025 - 11/16/2025</t>
+          <t>Levi Winslow Per diem for week of 11/10/2025 - 11/16/2025</t>
         </is>
       </c>
       <c r="G647" s="3" t="inlineStr">
@@ -24496,7 +24497,7 @@
         </is>
       </c>
       <c r="C648" s="5" t="n">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="D648" s="3" t="inlineStr">
         <is>
@@ -24510,7 +24511,7 @@
       </c>
       <c r="F648" s="3" t="inlineStr">
         <is>
-          <t>Levi Winslow Per diem for week of 11/10/2025 - 11/16/2025</t>
+          <t>Luke Giguere Per diem for week of 11/10/2025 - 11/16/2025</t>
         </is>
       </c>
       <c r="G648" s="3" t="inlineStr">
@@ -24546,7 +24547,7 @@
       </c>
       <c r="F649" s="3" t="inlineStr">
         <is>
-          <t>Luke Giguere Per diem for week of 11/10/2025 - 11/16/2025</t>
+          <t>Mike Cogswell Per diem for week of 11/10/2025 - 11/16/2025</t>
         </is>
       </c>
       <c r="G649" s="3" t="inlineStr">
@@ -24582,7 +24583,7 @@
       </c>
       <c r="F650" s="3" t="inlineStr">
         <is>
-          <t>Mike Cogswell Per diem for week of 11/10/2025 - 11/16/2025</t>
+          <t>Ryan Ordelt Per diem for week of 11/10/2025 - 11/16/2025</t>
         </is>
       </c>
       <c r="G650" s="3" t="inlineStr">
@@ -24600,30 +24601,30 @@
       </c>
       <c r="B651" s="3" t="inlineStr">
         <is>
-          <t>5108 · Meals &amp; entertainment (Direct)</t>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
         </is>
       </c>
       <c r="C651" s="5" t="n">
-        <v>350</v>
+        <v>31</v>
       </c>
       <c r="D651" s="3" t="inlineStr">
         <is>
-          <t>General Journal</t>
+          <t>Bill</t>
         </is>
       </c>
       <c r="E651" s="3" t="inlineStr">
         <is>
-          <t>16784</t>
+          <t>18585058</t>
         </is>
       </c>
       <c r="F651" s="3" t="inlineStr">
         <is>
-          <t>Ryan Ordelt Per diem for week of 11/10/2025 - 11/16/2025</t>
+          <t>NITRA pneumatic push-to-connect fitting</t>
         </is>
       </c>
       <c r="G651" s="3" t="inlineStr">
         <is>
-          <t>1006.2 · Calif B &amp; T Payroll Checking</t>
+          <t>2000 · Accounts Payable</t>
         </is>
       </c>
       <c r="H651" s="4" t="n">
@@ -24640,7 +24641,7 @@
         </is>
       </c>
       <c r="C652" s="5" t="n">
-        <v>31</v>
+        <v>2.42</v>
       </c>
       <c r="D652" s="3" t="inlineStr">
         <is>
@@ -24654,7 +24655,7 @@
       </c>
       <c r="F652" s="3" t="inlineStr">
         <is>
-          <t>NITRA pneumatic push-to-connect fitting</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="G652" s="3" t="inlineStr">
@@ -24668,7 +24669,7 @@
     </row>
     <row r="653">
       <c r="A653" s="2" t="n">
-        <v>45968</v>
+        <v>45971</v>
       </c>
       <c r="B653" s="3" t="inlineStr">
         <is>
@@ -24676,7 +24677,7 @@
         </is>
       </c>
       <c r="C653" s="5" t="n">
-        <v>2.42</v>
+        <v>451.08</v>
       </c>
       <c r="D653" s="3" t="inlineStr">
         <is>
@@ -24685,12 +24686,12 @@
       </c>
       <c r="E653" s="3" t="inlineStr">
         <is>
-          <t>18585058</t>
+          <t>93318089</t>
         </is>
       </c>
       <c r="F653" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>|BOLTPAK 5" RING 150 1/8" NAS</t>
         </is>
       </c>
       <c r="G653" s="3" t="inlineStr">
@@ -24712,7 +24713,7 @@
         </is>
       </c>
       <c r="C654" s="5" t="n">
-        <v>451.08</v>
+        <v>46.74</v>
       </c>
       <c r="D654" s="3" t="inlineStr">
         <is>
@@ -24726,7 +24727,7 @@
       </c>
       <c r="F654" s="3" t="inlineStr">
         <is>
-          <t>|BOLTPAK 5" RING 150 1/8" NAS</t>
+          <t>|BOLTPAK 2" RING 150 1/8" NAS</t>
         </is>
       </c>
       <c r="G654" s="3" t="inlineStr">
@@ -24748,7 +24749,7 @@
         </is>
       </c>
       <c r="C655" s="5" t="n">
-        <v>46.74</v>
+        <v>1044.8</v>
       </c>
       <c r="D655" s="3" t="inlineStr">
         <is>
@@ -24762,7 +24763,7 @@
       </c>
       <c r="F655" s="3" t="inlineStr">
         <is>
-          <t>|BOLTPAK 2" RING 150 1/8" NAS</t>
+          <t>|GATE VLV LF BRS 1" THD 200 F</t>
         </is>
       </c>
       <c r="G655" s="3" t="inlineStr">
@@ -24784,7 +24785,7 @@
         </is>
       </c>
       <c r="C656" s="5" t="n">
-        <v>1044.8</v>
+        <v>18.37</v>
       </c>
       <c r="D656" s="3" t="inlineStr">
         <is>
@@ -24793,12 +24794,12 @@
       </c>
       <c r="E656" s="3" t="inlineStr">
         <is>
-          <t>93318089</t>
+          <t>9705721745</t>
         </is>
       </c>
       <c r="F656" s="3" t="inlineStr">
         <is>
-          <t>|GATE VLV LF BRS 1" THD 200 F</t>
+          <t>VACUUM GAUGE,TEST,2 IN</t>
         </is>
       </c>
       <c r="G656" s="3" t="inlineStr">
@@ -24820,7 +24821,7 @@
         </is>
       </c>
       <c r="C657" s="5" t="n">
-        <v>18.37</v>
+        <v>1.42</v>
       </c>
       <c r="D657" s="3" t="inlineStr">
         <is>
@@ -24834,7 +24835,7 @@
       </c>
       <c r="F657" s="3" t="inlineStr">
         <is>
-          <t>VACUUM GAUGE,TEST,2 IN</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="G657" s="3" t="inlineStr">
@@ -24856,7 +24857,7 @@
         </is>
       </c>
       <c r="C658" s="5" t="n">
-        <v>1.42</v>
+        <v>40.84</v>
       </c>
       <c r="D658" s="3" t="inlineStr">
         <is>
@@ -24865,12 +24866,12 @@
       </c>
       <c r="E658" s="3" t="inlineStr">
         <is>
-          <t>9705721745</t>
+          <t>0935786</t>
         </is>
       </c>
       <c r="F658" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>2X20 FT PVC DWV S40 PE PIPE</t>
         </is>
       </c>
       <c r="G658" s="3" t="inlineStr">
@@ -24892,7 +24893,7 @@
         </is>
       </c>
       <c r="C659" s="5" t="n">
-        <v>40.84</v>
+        <v>80.65000000000001</v>
       </c>
       <c r="D659" s="3" t="inlineStr">
         <is>
@@ -24906,7 +24907,7 @@
       </c>
       <c r="F659" s="3" t="inlineStr">
         <is>
-          <t>2X20 FT PVC DWV S40 PE PIPE</t>
+          <t>3X20 FT PVC DWV S40 PE PIPE</t>
         </is>
       </c>
       <c r="G659" s="3" t="inlineStr">
@@ -24928,7 +24929,7 @@
         </is>
       </c>
       <c r="C660" s="5" t="n">
-        <v>80.65000000000001</v>
+        <v>109.54</v>
       </c>
       <c r="D660" s="3" t="inlineStr">
         <is>
@@ -24942,7 +24943,7 @@
       </c>
       <c r="F660" s="3" t="inlineStr">
         <is>
-          <t>3X20 FT PVC DWV S40 PE PIPE</t>
+          <t>LF 1-1/2 PXP COUP L/ST</t>
         </is>
       </c>
       <c r="G660" s="3" t="inlineStr">
@@ -24964,7 +24965,7 @@
         </is>
       </c>
       <c r="C661" s="5" t="n">
-        <v>109.54</v>
+        <v>206.66</v>
       </c>
       <c r="D661" s="3" t="inlineStr">
         <is>
@@ -24978,7 +24979,7 @@
       </c>
       <c r="F661" s="3" t="inlineStr">
         <is>
-          <t>LF 1-1/2 PXP COUP L/ST</t>
+          <t>6X20 FT PVC DWV S40 PE PIPE</t>
         </is>
       </c>
       <c r="G661" s="3" t="inlineStr">
@@ -25000,7 +25001,7 @@
         </is>
       </c>
       <c r="C662" s="5" t="n">
-        <v>206.66</v>
+        <v>287.8</v>
       </c>
       <c r="D662" s="3" t="inlineStr">
         <is>
@@ -25014,7 +25015,7 @@
       </c>
       <c r="F662" s="3" t="inlineStr">
         <is>
-          <t>6X20 FT PVC DWV S40 PE PIPE</t>
+          <t>6 PVC S40 SXS 90 ELL</t>
         </is>
       </c>
       <c r="G662" s="3" t="inlineStr">
@@ -25036,7 +25037,7 @@
         </is>
       </c>
       <c r="C663" s="5" t="n">
-        <v>287.8</v>
+        <v>27.22</v>
       </c>
       <c r="D663" s="3" t="inlineStr">
         <is>
@@ -25050,7 +25051,7 @@
       </c>
       <c r="F663" s="3" t="inlineStr">
         <is>
-          <t>6 PVC S40 SXS 90 ELL</t>
+          <t>6X4 PVC S40 SPXSLIP BUSH</t>
         </is>
       </c>
       <c r="G663" s="3" t="inlineStr">
@@ -25072,7 +25073,7 @@
         </is>
       </c>
       <c r="C664" s="5" t="n">
-        <v>27.22</v>
+        <v>64</v>
       </c>
       <c r="D664" s="3" t="inlineStr">
         <is>
@@ -25086,7 +25087,7 @@
       </c>
       <c r="F664" s="3" t="inlineStr">
         <is>
-          <t>6X4 PVC S40 SPXSLIP BUSH</t>
+          <t>6 PVC S40 SXM ADPT</t>
         </is>
       </c>
       <c r="G664" s="3" t="inlineStr">
@@ -25108,7 +25109,7 @@
         </is>
       </c>
       <c r="C665" s="5" t="n">
-        <v>64</v>
+        <v>90.42</v>
       </c>
       <c r="D665" s="3" t="inlineStr">
         <is>
@@ -25122,7 +25123,7 @@
       </c>
       <c r="F665" s="3" t="inlineStr">
         <is>
-          <t>6 PVC S40 SXM ADPT</t>
+          <t>6 PVC S40 SXSXS TEE</t>
         </is>
       </c>
       <c r="G665" s="3" t="inlineStr">
@@ -25144,7 +25145,7 @@
         </is>
       </c>
       <c r="C666" s="5" t="n">
-        <v>90.42</v>
+        <v>14.73</v>
       </c>
       <c r="D666" s="3" t="inlineStr">
         <is>
@@ -25158,7 +25159,7 @@
       </c>
       <c r="F666" s="3" t="inlineStr">
         <is>
-          <t>6 PVC S40 SXSXS TEE</t>
+          <t>4 PVC S80 VAN STONE SOC FLG</t>
         </is>
       </c>
       <c r="G666" s="3" t="inlineStr">
@@ -25180,7 +25181,7 @@
         </is>
       </c>
       <c r="C667" s="5" t="n">
-        <v>14.73</v>
+        <v>46.36</v>
       </c>
       <c r="D667" s="3" t="inlineStr">
         <is>
@@ -25194,7 +25195,7 @@
       </c>
       <c r="F667" s="3" t="inlineStr">
         <is>
-          <t>4 PVC S80 VAN STONE SOC FLG</t>
+          <t>6 PVC S80 VAN STONE SOC FLG</t>
         </is>
       </c>
       <c r="G667" s="3" t="inlineStr">
@@ -25216,7 +25217,7 @@
         </is>
       </c>
       <c r="C668" s="5" t="n">
-        <v>46.36</v>
+        <v>48.84</v>
       </c>
       <c r="D668" s="3" t="inlineStr">
         <is>
@@ -25230,7 +25231,7 @@
       </c>
       <c r="F668" s="3" t="inlineStr">
         <is>
-          <t>6 PVC S80 VAN STONE SOC FLG</t>
+          <t>6 150# ZN NA 1/16 RNG NBG SET</t>
         </is>
       </c>
       <c r="G668" s="3" t="inlineStr">
@@ -25252,7 +25253,7 @@
         </is>
       </c>
       <c r="C669" s="5" t="n">
-        <v>48.84</v>
+        <v>79.33</v>
       </c>
       <c r="D669" s="3" t="inlineStr">
         <is>
@@ -25266,7 +25267,7 @@
       </c>
       <c r="F669" s="3" t="inlineStr">
         <is>
-          <t>6 150# ZN NA 1/16 RNG NBG SET</t>
+          <t>Tax</t>
         </is>
       </c>
       <c r="G669" s="3" t="inlineStr">
@@ -25284,11 +25285,11 @@
       </c>
       <c r="B670" s="3" t="inlineStr">
         <is>
-          <t>5111 · Parts &amp; material costs (Direct)</t>
+          <t>5121 · Freight &amp; Shipping (Direct)</t>
         </is>
       </c>
       <c r="C670" s="5" t="n">
-        <v>79.33</v>
+        <v>330.75</v>
       </c>
       <c r="D670" s="3" t="inlineStr">
         <is>
@@ -25297,12 +25298,12 @@
       </c>
       <c r="E670" s="3" t="inlineStr">
         <is>
-          <t>0935786</t>
+          <t>93318089</t>
         </is>
       </c>
       <c r="F670" s="3" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>Shipping &amp; Handling</t>
         </is>
       </c>
       <c r="G670" s="3" t="inlineStr">
@@ -25316,15 +25317,15 @@
     </row>
     <row r="671">
       <c r="A671" s="2" t="n">
-        <v>45971</v>
+        <v>45972</v>
       </c>
       <c r="B671" s="3" t="inlineStr">
         <is>
-          <t>5121 · Freight &amp; Shipping (Direct)</t>
+          <t>5115 · Rent - Equipment (direct)</t>
         </is>
       </c>
       <c r="C671" s="5" t="n">
-        <v>330.75</v>
+        <v>2166</v>
       </c>
       <c r="D671" s="3" t="inlineStr">
         <is>
@@ -25333,12 +25334,12 @@
       </c>
       <c r="E671" s="3" t="inlineStr">
         <is>
-          <t>93318089</t>
+          <t>254738310-001</t>
         </is>
       </c>
       <c r="F671" s="3" t="inlineStr">
         <is>
-          <t>Shipping &amp; Handling</t>
+          <t>SKID STEER TRACK LOADER 1700-1999#</t>
         </is>
       </c>
       <c r="G671" s="3" t="inlineStr">
@@ -25360,7 +25361,7 @@
         </is>
       </c>
       <c r="C672" s="5" t="n">
-        <v>2166</v>
+        <v>540.5</v>
       </c>
       <c r="D672" s="3" t="inlineStr">
         <is>
@@ -25374,7 +25375,7 @@
       </c>
       <c r="F672" s="3" t="inlineStr">
         <is>
-          <t>SKID STEER TRACK LOADER 1700-1999#</t>
+          <t>Delivery &amp; Pickup</t>
         </is>
       </c>
       <c r="G672" s="3" t="inlineStr">
@@ -25396,7 +25397,7 @@
         </is>
       </c>
       <c r="C673" s="5" t="n">
-        <v>540.5</v>
+        <v>257.81</v>
       </c>
       <c r="D673" s="3" t="inlineStr">
         <is>
@@ -25410,7 +25411,7 @@
       </c>
       <c r="F673" s="3" t="inlineStr">
         <is>
-          <t>Delivery &amp; Pickup</t>
+          <t>Taxes &amp; Fees</t>
         </is>
       </c>
       <c r="G673" s="3" t="inlineStr">
@@ -25422,40 +25423,333 @@
         <v>400</v>
       </c>
     </row>
-    <row r="674">
-      <c r="A674" s="2" t="n">
-        <v>45972</v>
-      </c>
-      <c r="B674" s="3" t="inlineStr">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="40" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Account</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>1100 · Trade Debtors</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>186293.56</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>1504 · Undeposited Funds</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>186293.56</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>5004 · GTR  Cost of Sales - Parts</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Parts</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>37227.57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>5006 · Drilling Expense</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Outsource</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>330517.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>5105 · Travel - Airfare (Direct)</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>3234.92</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>5106 · Travel - Hotel (Direct)</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>45984.72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>5107 · Travel - Other (Direct)</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>2166.67</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>5107.1 · Travel - Car Rental</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>312.87</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>5108 · Meals &amp; entertainment (Direct)</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>23050</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>5111 · Parts &amp; material costs (Direct)</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Parts</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>106278.84</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>5113 · Repairs &amp; maint (Direct)</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Equipment</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>818.03</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
         <is>
           <t>5115 · Rent - Equipment (direct)</t>
         </is>
       </c>
-      <c r="C674" s="5" t="n">
-        <v>257.81</v>
-      </c>
-      <c r="D674" s="3" t="inlineStr">
-        <is>
-          <t>Bill</t>
-        </is>
-      </c>
-      <c r="E674" s="3" t="inlineStr">
-        <is>
-          <t>254738310-001</t>
-        </is>
-      </c>
-      <c r="F674" s="3" t="inlineStr">
-        <is>
-          <t>Taxes &amp; Fees</t>
-        </is>
-      </c>
-      <c r="G674" s="3" t="inlineStr">
-        <is>
-          <t>2000 · Accounts Payable</t>
-        </is>
-      </c>
-      <c r="H674" s="4" t="n">
-        <v>400</v>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Outsource</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>47077.67</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>5120 · Outside services (Direct)</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Outsource</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>149065.71</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>5121 · Freight &amp; Shipping (Direct)</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Outsource</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>17391.28</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>5122 · Motor vehicle exp (Direct)</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>580.9100000000001</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>5123 · Auto fuel (Direct)</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>1210.24</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>5128 · Health &amp; Safety Equip (Direct)</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Parts</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>295.4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>5129 · Misc expenses (Direct)</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Outsource</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>927.5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>6999 · Uncategorized Expenses</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="n">
+        <v>378.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>